<commit_message>
add updated time plan
</commit_message>
<xml_diff>
--- a/Zeitplan-uek-295.xlsx
+++ b/Zeitplan-uek-295.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukbe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukbe\uek-295\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8239AA8-5070-4E71-A200-EEDD88ECA3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B45EB0-B3A0-4219-AC97-85A88A9FFEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -265,18 +271,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -284,18 +298,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -688,7 +695,7 @@
   <dimension ref="A1:BY28"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BX25" sqref="BX25"/>
+      <selection activeCell="B28" sqref="B28:BE28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -700,22 +707,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -754,205 +761,205 @@
       <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:77" s="1" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>45601</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="20">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="14">
         <v>45602</v>
       </c>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
-      <c r="AO5" s="16"/>
-      <c r="AP5" s="16"/>
-      <c r="AQ5" s="16"/>
-      <c r="AR5" s="16"/>
-      <c r="AS5" s="16"/>
-      <c r="AT5" s="16"/>
-      <c r="AU5" s="16"/>
-      <c r="AV5" s="16"/>
-      <c r="AW5" s="16"/>
-      <c r="AX5" s="16"/>
-      <c r="AY5" s="16"/>
-      <c r="AZ5" s="16"/>
-      <c r="BA5" s="16"/>
-      <c r="BB5" s="16"/>
-      <c r="BC5" s="16"/>
-      <c r="BD5" s="16"/>
-      <c r="BE5" s="16"/>
-      <c r="BF5" s="16"/>
-      <c r="BG5" s="16"/>
-      <c r="BH5" s="16"/>
-      <c r="BI5" s="16"/>
-      <c r="BJ5" s="16"/>
-      <c r="BK5" s="16"/>
-      <c r="BL5" s="16"/>
-      <c r="BM5" s="16"/>
-      <c r="BN5" s="16"/>
-      <c r="BO5" s="16"/>
-      <c r="BP5" s="16"/>
-      <c r="BQ5" s="16"/>
-      <c r="BR5" s="16"/>
-      <c r="BS5" s="16"/>
-      <c r="BT5" s="16"/>
-      <c r="BU5" s="16"/>
-      <c r="BV5" s="16"/>
-      <c r="BW5" s="16"/>
-      <c r="BX5" s="16"/>
-      <c r="BY5" s="16"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="15"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="15"/>
+      <c r="AY5" s="15"/>
+      <c r="AZ5" s="15"/>
+      <c r="BA5" s="15"/>
+      <c r="BB5" s="15"/>
+      <c r="BC5" s="15"/>
+      <c r="BD5" s="15"/>
+      <c r="BE5" s="15"/>
+      <c r="BF5" s="15"/>
+      <c r="BG5" s="15"/>
+      <c r="BH5" s="15"/>
+      <c r="BI5" s="15"/>
+      <c r="BJ5" s="15"/>
+      <c r="BK5" s="15"/>
+      <c r="BL5" s="15"/>
+      <c r="BM5" s="15"/>
+      <c r="BN5" s="15"/>
+      <c r="BO5" s="15"/>
+      <c r="BP5" s="15"/>
+      <c r="BQ5" s="15"/>
+      <c r="BR5" s="15"/>
+      <c r="BS5" s="15"/>
+      <c r="BT5" s="15"/>
+      <c r="BU5" s="15"/>
+      <c r="BV5" s="15"/>
+      <c r="BW5" s="15"/>
+      <c r="BX5" s="15"/>
+      <c r="BY5" s="15"/>
     </row>
     <row r="6" spans="1:77" s="1" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15" t="s">
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15" t="s">
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15" t="s">
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15" t="s">
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15" t="s">
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15" t="s">
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15" t="s">
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AO6" s="16"/>
+      <c r="AP6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15" t="s">
+      <c r="AQ6" s="16"/>
+      <c r="AR6" s="16"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15" t="s">
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="16"/>
+      <c r="AW6" s="16"/>
+      <c r="AX6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-      <c r="BB6" s="15" t="s">
+      <c r="AY6" s="16"/>
+      <c r="AZ6" s="16"/>
+      <c r="BA6" s="16"/>
+      <c r="BB6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="BC6" s="15"/>
-      <c r="BD6" s="15"/>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="15"/>
-      <c r="BG6" s="15"/>
-      <c r="BH6" s="15"/>
-      <c r="BI6" s="15"/>
-      <c r="BJ6" s="15"/>
-      <c r="BK6" s="15"/>
-      <c r="BL6" s="15"/>
-      <c r="BM6" s="15"/>
-      <c r="BN6" s="15"/>
-      <c r="BO6" s="15"/>
-      <c r="BP6" s="15"/>
-      <c r="BQ6" s="15"/>
-      <c r="BR6" s="15"/>
-      <c r="BS6" s="15"/>
-      <c r="BT6" s="15"/>
-      <c r="BU6" s="15"/>
-      <c r="BV6" s="15"/>
-      <c r="BW6" s="15"/>
-      <c r="BX6" s="15"/>
-      <c r="BY6" s="15"/>
+      <c r="BC6" s="16"/>
+      <c r="BD6" s="16"/>
+      <c r="BE6" s="16"/>
+      <c r="BF6" s="16"/>
+      <c r="BG6" s="16"/>
+      <c r="BH6" s="16"/>
+      <c r="BI6" s="16"/>
+      <c r="BJ6" s="16"/>
+      <c r="BK6" s="16"/>
+      <c r="BL6" s="16"/>
+      <c r="BM6" s="16"/>
+      <c r="BN6" s="16"/>
+      <c r="BO6" s="16"/>
+      <c r="BP6" s="16"/>
+      <c r="BQ6" s="16"/>
+      <c r="BR6" s="16"/>
+      <c r="BS6" s="16"/>
+      <c r="BT6" s="16"/>
+      <c r="BU6" s="16"/>
+      <c r="BV6" s="16"/>
+      <c r="BW6" s="16"/>
+      <c r="BX6" s="16"/>
+      <c r="BY6" s="16"/>
     </row>
     <row r="7" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1029,8 +1036,8 @@
       <c r="BY7" s="6"/>
     </row>
     <row r="8" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
@@ -1108,28 +1115,28 @@
       <c r="BY8" s="6"/>
     </row>
     <row r="9" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
       <c r="U9" s="7"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -1189,28 +1196,28 @@
       <c r="BY9" s="6"/>
     </row>
     <row r="10" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
@@ -1268,7 +1275,7 @@
       <c r="BY10" s="6"/>
     </row>
     <row r="11" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="7"/>
@@ -1290,13 +1297,13 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
@@ -1349,7 +1356,7 @@
       <c r="BY11" s="7"/>
     </row>
     <row r="12" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="7"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1371,10 +1378,10 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
@@ -1428,7 +1435,7 @@
       <c r="BY12" s="7"/>
     </row>
     <row r="13" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="7"/>
@@ -1455,10 +1462,10 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
-      <c r="Z13" s="17"/>
-      <c r="AA13" s="17"/>
-      <c r="AB13" s="17"/>
-      <c r="AC13" s="17"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
@@ -1509,7 +1516,7 @@
       <c r="BY13" s="7"/>
     </row>
     <row r="14" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="7"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1535,11 +1542,11 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
       <c r="AF14" s="6"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="6"/>
@@ -1588,7 +1595,7 @@
       <c r="BY14" s="7"/>
     </row>
     <row r="15" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="7"/>
@@ -1619,14 +1626,14 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="6"/>
-      <c r="AD15" s="17"/>
-      <c r="AE15" s="17"/>
-      <c r="AF15" s="17"/>
-      <c r="AG15" s="17"/>
-      <c r="AH15" s="17"/>
-      <c r="AI15" s="17"/>
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
       <c r="AL15" s="6"/>
       <c r="AM15" s="6"/>
       <c r="AN15" s="6"/>
@@ -1669,7 +1676,7 @@
       <c r="BY15" s="7"/>
     </row>
     <row r="16" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="7"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1700,14 +1707,14 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="7"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
-      <c r="AL16" s="6"/>
-      <c r="AM16" s="6"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="20"/>
+      <c r="AL16" s="20"/>
+      <c r="AM16" s="20"/>
       <c r="AN16" s="6"/>
       <c r="AO16" s="6"/>
       <c r="AP16" s="6"/>
@@ -1748,7 +1755,7 @@
       <c r="BY16" s="7"/>
     </row>
     <row r="17" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="7"/>
@@ -1787,10 +1794,10 @@
       <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="6"/>
-      <c r="AL17" s="17"/>
-      <c r="AM17" s="17"/>
-      <c r="AN17" s="17"/>
-      <c r="AO17" s="17"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
+      <c r="AN17" s="9"/>
+      <c r="AO17" s="9"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="6"/>
       <c r="AR17" s="6"/>
@@ -1829,7 +1836,7 @@
       <c r="BY17" s="7"/>
     </row>
     <row r="18" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="7"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1868,8 +1875,8 @@
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
       <c r="AM18" s="6"/>
-      <c r="AN18" s="6"/>
-      <c r="AO18" s="6"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="20"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
       <c r="AR18" s="7"/>
@@ -1908,7 +1915,7 @@
       <c r="BY18" s="7"/>
     </row>
     <row r="19" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="7"/>
@@ -1953,10 +1960,10 @@
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
-      <c r="AR19" s="17"/>
-      <c r="AS19" s="17"/>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
+      <c r="AR19" s="9"/>
+      <c r="AS19" s="9"/>
+      <c r="AT19" s="9"/>
+      <c r="AU19" s="9"/>
       <c r="AV19" s="6"/>
       <c r="AW19" s="6"/>
       <c r="AX19" s="6"/>
@@ -1989,7 +1996,7 @@
       <c r="BY19" s="7"/>
     </row>
     <row r="20" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="7"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -2032,8 +2039,8 @@
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="6"/>
-      <c r="AR20" s="6"/>
-      <c r="AS20" s="6"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="20"/>
       <c r="AT20" s="6"/>
       <c r="AU20" s="6"/>
       <c r="AV20" s="6"/>
@@ -2068,7 +2075,7 @@
       <c r="BY20" s="7"/>
     </row>
     <row r="21" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="7"/>
@@ -2117,7 +2124,7 @@
       <c r="AS21" s="6"/>
       <c r="AT21" s="6"/>
       <c r="AU21" s="6"/>
-      <c r="AV21" s="19"/>
+      <c r="AV21" s="11"/>
       <c r="AW21" s="6"/>
       <c r="AX21" s="6"/>
       <c r="AY21" s="6"/>
@@ -2149,7 +2156,7 @@
       <c r="BY21" s="7"/>
     </row>
     <row r="22" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="7"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -2194,8 +2201,8 @@
       <c r="AQ22" s="6"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="6"/>
-      <c r="AT22" s="6"/>
-      <c r="AU22" s="6"/>
+      <c r="AT22" s="20"/>
+      <c r="AU22" s="20"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="6"/>
       <c r="AX22" s="6"/>
@@ -2228,7 +2235,7 @@
       <c r="BY22" s="7"/>
     </row>
     <row r="23" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="7"/>
@@ -2278,9 +2285,9 @@
       <c r="AT23" s="6"/>
       <c r="AU23" s="6"/>
       <c r="AV23" s="6"/>
-      <c r="AW23" s="17"/>
-      <c r="AX23" s="17"/>
-      <c r="AY23" s="17"/>
+      <c r="AW23" s="9"/>
+      <c r="AX23" s="9"/>
+      <c r="AY23" s="9"/>
       <c r="AZ23" s="6"/>
       <c r="BA23" s="6"/>
       <c r="BB23" s="6"/>
@@ -2309,7 +2316,7 @@
       <c r="BY23" s="7"/>
     </row>
     <row r="24" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="7"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2356,8 +2363,8 @@
       <c r="AS24" s="6"/>
       <c r="AT24" s="6"/>
       <c r="AU24" s="6"/>
-      <c r="AV24" s="6"/>
-      <c r="AW24" s="6"/>
+      <c r="AV24" s="20"/>
+      <c r="AW24" s="20"/>
       <c r="AX24" s="6"/>
       <c r="AY24" s="6"/>
       <c r="AZ24" s="6"/>
@@ -2388,7 +2395,7 @@
       <c r="BY24" s="7"/>
     </row>
     <row r="25" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="7"/>
@@ -2441,8 +2448,8 @@
       <c r="AW25" s="6"/>
       <c r="AX25" s="6"/>
       <c r="AY25" s="6"/>
-      <c r="AZ25" s="17"/>
-      <c r="BA25" s="17"/>
+      <c r="AZ25" s="9"/>
+      <c r="BA25" s="9"/>
       <c r="BB25" s="6"/>
       <c r="BC25" s="6"/>
       <c r="BD25" s="6"/>
@@ -2465,11 +2472,11 @@
       <c r="BU25" s="7"/>
       <c r="BV25" s="7"/>
       <c r="BW25" s="7"/>
-      <c r="BX25" s="7"/>
+      <c r="BX25" s="20"/>
       <c r="BY25" s="7"/>
     </row>
     <row r="26" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="7"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -2518,8 +2525,8 @@
       <c r="AU26" s="6"/>
       <c r="AV26" s="6"/>
       <c r="AW26" s="6"/>
-      <c r="AX26" s="6"/>
-      <c r="AY26" s="6"/>
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
       <c r="AZ26" s="6"/>
       <c r="BA26" s="6"/>
       <c r="BB26" s="6"/>
@@ -2548,65 +2555,65 @@
       <c r="BY26" s="7"/>
     </row>
     <row r="27" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="17"/>
-      <c r="AB27" s="17"/>
-      <c r="AC27" s="17"/>
-      <c r="AD27" s="17"/>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="17"/>
-      <c r="AH27" s="17"/>
-      <c r="AI27" s="17"/>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="17"/>
-      <c r="AM27" s="17"/>
-      <c r="AN27" s="17"/>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="17"/>
-      <c r="AR27" s="17"/>
-      <c r="AS27" s="17"/>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="17"/>
-      <c r="AW27" s="17"/>
-      <c r="AX27" s="17"/>
-      <c r="AY27" s="17"/>
-      <c r="AZ27" s="17"/>
-      <c r="BA27" s="17"/>
-      <c r="BB27" s="17"/>
-      <c r="BC27" s="17"/>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="17"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="9"/>
+      <c r="AL27" s="9"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="9"/>
+      <c r="AO27" s="9"/>
+      <c r="AP27" s="9"/>
+      <c r="AQ27" s="9"/>
+      <c r="AR27" s="9"/>
+      <c r="AS27" s="9"/>
+      <c r="AT27" s="9"/>
+      <c r="AU27" s="9"/>
+      <c r="AV27" s="9"/>
+      <c r="AW27" s="9"/>
+      <c r="AX27" s="9"/>
+      <c r="AY27" s="9"/>
+      <c r="AZ27" s="9"/>
+      <c r="BA27" s="9"/>
+      <c r="BB27" s="9"/>
+      <c r="BC27" s="9"/>
+      <c r="BD27" s="9"/>
+      <c r="BE27" s="9"/>
       <c r="BF27" s="6"/>
       <c r="BG27" s="6"/>
       <c r="BH27" s="6"/>
@@ -2629,63 +2636,63 @@
       <c r="BY27" s="7"/>
     </row>
     <row r="28" spans="1:77" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="6"/>
-      <c r="AG28" s="7"/>
-      <c r="AH28" s="6"/>
-      <c r="AI28" s="6"/>
-      <c r="AJ28" s="6"/>
-      <c r="AK28" s="6"/>
-      <c r="AL28" s="6"/>
-      <c r="AM28" s="6"/>
-      <c r="AN28" s="6"/>
-      <c r="AO28" s="6"/>
-      <c r="AP28" s="6"/>
-      <c r="AQ28" s="6"/>
-      <c r="AR28" s="6"/>
-      <c r="AS28" s="6"/>
-      <c r="AT28" s="6"/>
-      <c r="AU28" s="6"/>
-      <c r="AV28" s="6"/>
-      <c r="AW28" s="6"/>
-      <c r="AX28" s="6"/>
-      <c r="AY28" s="6"/>
-      <c r="AZ28" s="6"/>
-      <c r="BA28" s="6"/>
-      <c r="BB28" s="6"/>
-      <c r="BC28" s="6"/>
-      <c r="BD28" s="6"/>
-      <c r="BE28" s="6"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20"/>
+      <c r="AE28" s="20"/>
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="20"/>
+      <c r="AH28" s="20"/>
+      <c r="AI28" s="20"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20"/>
+      <c r="AN28" s="20"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20"/>
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20"/>
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
+      <c r="BB28" s="20"/>
+      <c r="BC28" s="20"/>
+      <c r="BD28" s="20"/>
+      <c r="BE28" s="20"/>
       <c r="BF28" s="6"/>
       <c r="BG28" s="6"/>
       <c r="BH28" s="6"/>
@@ -2709,20 +2716,13 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="N5:AC5"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="BF6:BI6"/>
+    <mergeCell ref="BJ6:BM6"/>
+    <mergeCell ref="BN6:BQ6"/>
+    <mergeCell ref="BB6:BE6"/>
+    <mergeCell ref="AT6:AW6"/>
     <mergeCell ref="AD5:AS5"/>
     <mergeCell ref="AT5:BM5"/>
     <mergeCell ref="BN5:BY5"/>
@@ -2733,19 +2733,26 @@
     <mergeCell ref="AH6:AK6"/>
     <mergeCell ref="AL6:AO6"/>
     <mergeCell ref="AP6:AS6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="BF6:BI6"/>
-    <mergeCell ref="BJ6:BM6"/>
-    <mergeCell ref="BN6:BQ6"/>
     <mergeCell ref="BR6:BU6"/>
     <mergeCell ref="BV6:BY6"/>
-    <mergeCell ref="BB6:BE6"/>
-    <mergeCell ref="AT6:AW6"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="N5:AC5"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.31496062992125984"/>

</xml_diff>